<commit_message>
ej 2 y 3
</commit_message>
<xml_diff>
--- a/Practicos/practico6.xlsx
+++ b/Practicos/practico6.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="19245" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="19245" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -353,12 +354,13 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <legacyDrawing r:id="rId1"/>
   <oleObjects>
     <oleObject progId="Equation.DSMT4" shapeId="1025" r:id="rId2"/>
@@ -370,7 +372,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21:D22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
@@ -381,6 +385,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <legacyDrawing r:id="rId1"/>
+  <oleObjects>
+    <oleObject progId="Equation.DSMT4" shapeId="2049" r:id="rId2"/>
+  </oleObjects>
 </worksheet>
 </file>
 
@@ -388,10 +397,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <oleObjects>
+    <oleObject progId="Equation.DSMT4" shapeId="3073" r:id="rId2"/>
+  </oleObjects>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
libro y guia 6
</commit_message>
<xml_diff>
--- a/Practicos/practico6.xlsx
+++ b/Practicos/practico6.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="19245" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="19245" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -17,9 +18,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>G</t>
+  </si>
+  <si>
+    <t>a)</t>
+  </si>
+  <si>
+    <t>b)</t>
+  </si>
+  <si>
+    <t>c)</t>
   </si>
 </sst>
 </file>
@@ -395,6 +405,42 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="D1:D25"/>
+  <sheetViews>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="4:4">
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4">
+      <c r="D17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="4:4">
+      <c r="D25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <legacyDrawing r:id="rId1"/>
+  <oleObjects>
+    <oleObject progId="Equation.DSMT4" shapeId="3074" r:id="rId2"/>
+    <oleObject progId="Equation.DSMT4" shapeId="3075" r:id="rId3"/>
+  </oleObjects>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -404,7 +450,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
   <oleObjects>
-    <oleObject progId="Equation.DSMT4" shapeId="3073" r:id="rId2"/>
+    <oleObject progId="Equation.DSMT4" shapeId="4097" r:id="rId2"/>
   </oleObjects>
 </worksheet>
 </file>
</xml_diff>